<commit_message>
Finished the first edition.
</commit_message>
<xml_diff>
--- a/document/paper/model-compare.xlsx
+++ b/document/paper/model-compare.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="-19440" yWindow="-320" windowWidth="18640" windowHeight="18560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="108">
   <si>
     <t>RGB</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -912,6 +913,85 @@
       </rPr>
       <t>（动态混合贝叶斯模型）</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Person</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>Precision (%)</t>
+  </si>
+  <si>
+    <t>Recall (%)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>本文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Ni, Moulin, Yan, ECCV 2012 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Sung et al., AAAI PAIR 2011, ICRA 2012. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Piyathilaka, Kodagoda, ICIEA 2013 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Yang, Tian, JVCIR 2013 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Wang et al., PAMI 2013 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Ni et al., Cybernetics 2013 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaglio, Lo Re, Morana, HMS 2014 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gupta, Chia, Rajan, MM 2013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Koppula, Gupta, Saxena, IJRR 2012. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Zhang, Tian, NWPJ 2012 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Faria, Premebida, Nunes, RO-MAN 2014 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Parisi, Weber, Wermter, Front. Neurobot. 2015 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Zhu, Chen, Guo, IVC 2014 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Shan, Akella, ARSO 2014 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -999,8 +1079,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1040,7 +1122,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -1050,6 +1132,7 @@
     <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1058,6 +1141,7 @@
     <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1388,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1433,61 +1517,63 @@
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="78">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4">
-        <v>0.78200000000000003</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0.78200000000000003</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>25</v>
+      <c r="E2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="7">
+        <v>0.69</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="J2" s="2">
+        <v>2011</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="65">
       <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.91100000000000003</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.91900000000000004</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0.91900000000000004</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>26</v>
+        <v>56</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2013</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="101">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1495,451 +1581,442 @@
         <v>6</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.91059999999999997</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.91869999999999996</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="2" t="s">
-        <v>27</v>
+        <v>83</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3">
+        <v>0.747</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="65">
-      <c r="A5" s="6" t="s">
-        <v>16</v>
+      <c r="A5" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="F5" s="4" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="H5" s="4">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.78200000000000003</v>
+      </c>
       <c r="J5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="55">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0.66600000000000004</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="2" t="s">
-        <v>30</v>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="7">
+        <v>0.86</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.84</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2014</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" ht="52">
       <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="C7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G7" s="3">
-        <v>0.93200000000000005</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="H7" s="3">
-        <v>0.84599999999999997</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.875</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>31</v>
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="78">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0.78</v>
-      </c>
-      <c r="I8" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.875</v>
+      </c>
       <c r="J8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="156">
       <c r="A9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="1">
-        <v>2009</v>
-      </c>
+      <c r="I9" s="3">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="78">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="E10" s="4" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.91900000000000004</v>
+      </c>
       <c r="J10" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" ht="30">
       <c r="A11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="F11" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2011</v>
+      </c>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="69">
       <c r="A12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="E12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="7">
-        <v>0.69</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.57299999999999995</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.64200000000000002</v>
-      </c>
-      <c r="J12" s="2">
-        <v>2011</v>
+        <v>86</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.91059999999999997</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.91869999999999996</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="78">
-      <c r="A13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="4"/>
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="C13" s="4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0.754</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="78">
       <c r="A14" s="4" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.77300000000000002</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0.76700000000000002</v>
+        <v>19</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.66600000000000004</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="80">
       <c r="A15" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0.747</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0.78</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="43">
       <c r="A16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>47</v>
+        <v>80</v>
+      </c>
+      <c r="J16" s="1">
+        <v>2009</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="28">
       <c r="A17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="I17" s="7">
-        <v>0.87</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="52">
       <c r="A18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="52">
       <c r="A19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0.88400000000000001</v>
+        <v>74</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.754</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="39">
       <c r="A20" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="E20" s="4" t="s">
-        <v>56</v>
+        <v>81</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="G20" s="3">
-        <v>0.75900000000000001</v>
+        <v>0.77300000000000002</v>
       </c>
       <c r="H20" s="3">
-        <v>0.69499999999999995</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="J20" s="1">
-        <v>2013</v>
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="26">
       <c r="A21" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="E21" s="4" t="s">
-        <v>60</v>
+        <v>84</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="39">
       <c r="A22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="7">
-        <v>0.86</v>
-      </c>
-      <c r="H22" s="7">
-        <v>0.84</v>
-      </c>
-      <c r="I22" s="3">
-        <v>0.81899999999999995</v>
-      </c>
-      <c r="J22" s="1">
-        <v>2014</v>
+        <v>51</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="52">
       <c r="A23" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C23" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="E23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="J23" s="1">
-        <v>2011</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="121">
@@ -1954,6 +2031,220 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:J24">
+    <sortCondition ref="I1"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="52" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3">
+        <v>93.8</v>
+      </c>
+      <c r="C3">
+        <v>94.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4">
+        <v>93.2</v>
+      </c>
+      <c r="C4">
+        <v>84.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5">
+        <v>91.9</v>
+      </c>
+      <c r="C5">
+        <v>90.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6">
+        <v>91.1</v>
+      </c>
+      <c r="C6">
+        <v>91.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7">
+        <v>86</v>
+      </c>
+      <c r="C7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8">
+        <v>81.8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9">
+        <v>80.8</v>
+      </c>
+      <c r="C9">
+        <v>71.400000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="C10">
+        <v>75.400000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11">
+        <v>77.3</v>
+      </c>
+      <c r="C11">
+        <v>76.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="C12">
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13">
+        <v>74.7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="C14">
+        <v>66.599999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15">
+        <v>70</v>
+      </c>
+      <c r="C15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="C16">
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17">
+        <v>65.319999999999993</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A3:C17">
+    <sortCondition descending="1" ref="B3"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>